<commit_message>
Sprint 2 Updated File
</commit_message>
<xml_diff>
--- a/files/Documents/Team 3 Documents/xslxnoPII.xlsx
+++ b/files/Documents/Team 3 Documents/xslxnoPII.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f80bfed2d9b5c5a/Documents/GitHub/comp410_summer_2022/.github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\audri\Documents\comp410\comp410_summer_2022\files\Documents\Team 3 Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACCE6D36-1546-421E-9B42-D6996CD4D4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360A741-4B22-44CB-B822-6A837E049AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F115AE3B-8BD7-478F-948A-D20875E4FF2C}"/>
+    <workbookView xWindow="1185" yWindow="3990" windowWidth="15375" windowHeight="7875" xr2:uid="{F115AE3B-8BD7-478F-948A-D20875E4FF2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>